<commit_message>
add the root part
</commit_message>
<xml_diff>
--- a/data/course_list.xlsx
+++ b/data/course_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huangjiani/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huangjiani/CourseSelectionSystem/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6836931A-0667-1E45-8481-9E17A85EA8A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB7E182C-67C3-2443-811B-0AF869D1AF00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3140" yWindow="460" windowWidth="28040" windowHeight="16420" xr2:uid="{A2DB1C49-99E9-1748-A5CF-F168FA39BF00}"/>
+    <workbookView xWindow="3780" yWindow="7840" windowWidth="28040" windowHeight="16420" xr2:uid="{39529C12-9FE3-5F4E-B7B9-7505A7E094E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>course_id</t>
   </si>
   <si>
-    <t>section_id</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
@@ -48,43 +45,22 @@
     <t>dept_name</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>classroom_no</t>
-  </si>
-  <si>
-    <t>lesson</t>
-  </si>
-  <si>
-    <t>limit</t>
-  </si>
-  <si>
-    <t>day</t>
-  </si>
-  <si>
-    <t>instructor_id</t>
-  </si>
-  <si>
-    <t>WHIT00001</t>
-  </si>
-  <si>
-    <t>白色相簿</t>
-  </si>
-  <si>
-    <t>白学系</t>
-  </si>
-  <si>
-    <t>HGX222</t>
-  </si>
-  <si>
-    <t>LAWS00000005</t>
-  </si>
-  <si>
-    <t>HGX223</t>
-  </si>
-  <si>
-    <t>4-5</t>
+    <t>CCCC120001</t>
+  </si>
+  <si>
+    <t>我不做人了</t>
+  </si>
+  <si>
+    <t>软件学院</t>
+  </si>
+  <si>
+    <t>DDDD111111</t>
+  </si>
+  <si>
+    <t>我死了</t>
+  </si>
+  <si>
+    <t>计算机学院</t>
   </si>
 </sst>
 </file>
@@ -120,9 +96,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,121 +411,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26ED6A3F-9078-4342-889C-D8C333065B99}">
-  <dimension ref="A1:K3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A48145-9049-5946-BC82-B4D8D35E90CE}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="11" max="11" width="15.6640625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="I2">
-        <v>20</v>
-      </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-      <c r="K2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>20</v>
-      </c>
-      <c r="J3">
-        <v>3</v>
-      </c>
-      <c r="K3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>